<commit_message>
End of week push
Main work was developing fleet optimization (transportation folder), still under development
</commit_message>
<xml_diff>
--- a/productionOptModel/dataInputs/inputSheet.xlsx
+++ b/productionOptModel/dataInputs/inputSheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\KAUST\productionOptModel\dataInputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{373D94E5-5104-43BF-B92F-16EFA1406483}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{844BED11-96DE-42AA-89A4-68BC6C73CE12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6763" yWindow="3206" windowWidth="24686" windowHeight="9565" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4251" yWindow="3540" windowWidth="24686" windowHeight="9454" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="systemSettings" sheetId="1" r:id="rId1"/>
@@ -730,8 +730,8 @@
   </sheetPr>
   <dimension ref="A1:F40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -765,8 +765,8 @@
         <v>14</v>
       </c>
       <c r="B2" s="5">
-        <f>200*1000</f>
-        <v>200000</v>
+        <f>3288*1000</f>
+        <v>3288000</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>61</v>

</xml_diff>